<commit_message>
ready to regenerate navigation and authorization after markdown changes for columns and models
</commit_message>
<xml_diff>
--- a/rights.xlsx
+++ b/rights.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="16340" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="developer" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="129">
   <si>
     <t>developer</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>edit own details</t>
+  </si>
+  <si>
+    <t>Column</t>
   </si>
 </sst>
 </file>
@@ -483,8 +486,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -582,7 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -629,6 +634,7 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -675,6 +681,7 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1004,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1028,7 +1035,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1036,7 +1043,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1044,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1052,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1060,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1068,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1076,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1084,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1092,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1100,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1108,12 +1115,20 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B1:B12">
-    <sortCondition ref="B12"/>
+  <sortState ref="A1:B13">
+    <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1263,7 +1278,6 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1292,7 +1306,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1515,7 +1528,6 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2069,7 +2081,6 @@
     <sortCondition ref="A26"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2153,7 +2164,6 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2166,14 +2176,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
prior to adding ActiveRecord beforeValidate to deal with populating null values automatically where possible - particularly when used only to enforce referencial integrity.
</commit_message>
<xml_diff>
--- a/rights.xlsx
+++ b/rights.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="760" windowWidth="25360" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="2880" yWindow="260" windowWidth="25360" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_auth_item_child" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="312">
   <si>
     <t>Account</t>
   </si>
@@ -1369,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B223"/>
+  <dimension ref="A1:B224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2271,10 +2271,10 @@
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B112" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>209</v>
       </c>
       <c r="B113" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>209</v>
       </c>
       <c r="B114" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2298,7 +2298,7 @@
         <v>209</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2306,39 +2306,39 @@
         <v>209</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B118" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B119" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B120" t="s">
-        <v>111</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2346,7 +2346,7 @@
         <v>209</v>
       </c>
       <c r="B121" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2354,7 +2354,7 @@
         <v>209</v>
       </c>
       <c r="B122" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2362,31 +2362,31 @@
         <v>209</v>
       </c>
       <c r="B123" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B124" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B125" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B126" t="s">
-        <v>116</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2394,23 +2394,23 @@
         <v>209</v>
       </c>
       <c r="B127" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B128" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B129" t="s">
-        <v>118</v>
+        <v>15</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2418,7 +2418,7 @@
         <v>209</v>
       </c>
       <c r="B130" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2426,7 +2426,7 @@
         <v>209</v>
       </c>
       <c r="B131" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2434,15 +2434,15 @@
         <v>209</v>
       </c>
       <c r="B132" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B133" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2450,55 +2450,55 @@
         <v>207</v>
       </c>
       <c r="B134" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B135" t="s">
-        <v>123</v>
+        <v>20</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B136" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B137" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B138" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B139" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B140" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2506,23 +2506,23 @@
         <v>209</v>
       </c>
       <c r="B141" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B142" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B143" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2530,7 +2530,7 @@
         <v>209</v>
       </c>
       <c r="B144" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2538,7 +2538,7 @@
         <v>209</v>
       </c>
       <c r="B145" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2546,7 +2546,7 @@
         <v>209</v>
       </c>
       <c r="B146" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2554,7 +2554,7 @@
         <v>209</v>
       </c>
       <c r="B147" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2562,7 +2562,7 @@
         <v>209</v>
       </c>
       <c r="B148" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2570,7 +2570,7 @@
         <v>209</v>
       </c>
       <c r="B149" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2578,7 +2578,7 @@
         <v>209</v>
       </c>
       <c r="B150" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2586,39 +2586,39 @@
         <v>209</v>
       </c>
       <c r="B151" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B152" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B153" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B154" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B155" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2626,7 +2626,7 @@
         <v>206</v>
       </c>
       <c r="B156" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2634,7 +2634,7 @@
         <v>206</v>
       </c>
       <c r="B157" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2642,15 +2642,15 @@
         <v>206</v>
       </c>
       <c r="B158" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B159" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2658,15 +2658,15 @@
         <v>211</v>
       </c>
       <c r="B160" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B161" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2674,7 +2674,7 @@
         <v>206</v>
       </c>
       <c r="B162" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2682,15 +2682,15 @@
         <v>206</v>
       </c>
       <c r="B163" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B164" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2698,7 +2698,7 @@
         <v>211</v>
       </c>
       <c r="B165" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2706,7 +2706,7 @@
         <v>211</v>
       </c>
       <c r="B166" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2714,7 +2714,7 @@
         <v>211</v>
       </c>
       <c r="B167" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2722,7 +2722,7 @@
         <v>211</v>
       </c>
       <c r="B168" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2730,79 +2730,79 @@
         <v>211</v>
       </c>
       <c r="B169" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B170" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B171" t="s">
-        <v>158</v>
+        <v>55</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B172" t="s">
-        <v>56</v>
+        <v>158</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B173" t="s">
-        <v>159</v>
+        <v>56</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B174" t="s">
-        <v>57</v>
+        <v>159</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B175" t="s">
-        <v>160</v>
+        <v>57</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B176" t="s">
-        <v>58</v>
+        <v>160</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B177" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B178" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2810,7 +2810,7 @@
         <v>209</v>
       </c>
       <c r="B179" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2818,7 +2818,7 @@
         <v>209</v>
       </c>
       <c r="B180" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2826,7 +2826,7 @@
         <v>209</v>
       </c>
       <c r="B181" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2834,7 +2834,7 @@
         <v>209</v>
       </c>
       <c r="B182" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2842,7 +2842,7 @@
         <v>209</v>
       </c>
       <c r="B183" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2850,15 +2850,15 @@
         <v>209</v>
       </c>
       <c r="B184" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B185" t="s">
-        <v>170</v>
+        <v>66</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -2866,20 +2866,20 @@
         <v>211</v>
       </c>
       <c r="B186" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B187" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B188" t="s">
         <v>69</v>
@@ -2887,26 +2887,26 @@
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B189" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B190" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B191" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -2914,23 +2914,23 @@
         <v>211</v>
       </c>
       <c r="B192" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B193" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B194" t="s">
-        <v>177</v>
+        <v>74</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -2938,7 +2938,7 @@
         <v>211</v>
       </c>
       <c r="B195" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2946,7 +2946,7 @@
         <v>211</v>
       </c>
       <c r="B196" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2954,7 +2954,7 @@
         <v>211</v>
       </c>
       <c r="B197" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -2962,7 +2962,7 @@
         <v>211</v>
       </c>
       <c r="B198" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2970,7 +2970,7 @@
         <v>211</v>
       </c>
       <c r="B199" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2978,23 +2978,23 @@
         <v>211</v>
       </c>
       <c r="B200" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B201" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B202" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -3002,7 +3002,7 @@
         <v>211</v>
       </c>
       <c r="B203" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -3010,7 +3010,7 @@
         <v>211</v>
       </c>
       <c r="B204" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -3018,15 +3018,15 @@
         <v>211</v>
       </c>
       <c r="B205" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B206" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -3034,28 +3034,28 @@
         <v>209</v>
       </c>
       <c r="B207" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B208" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B209" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B210" t="s">
         <v>89</v>
@@ -3066,7 +3066,7 @@
         <v>211</v>
       </c>
       <c r="B211" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -3074,7 +3074,7 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -3082,7 +3082,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -3090,7 +3090,7 @@
         <v>211</v>
       </c>
       <c r="B214" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -3098,7 +3098,7 @@
         <v>211</v>
       </c>
       <c r="B215" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -3106,7 +3106,7 @@
         <v>211</v>
       </c>
       <c r="B216" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -3114,7 +3114,7 @@
         <v>211</v>
       </c>
       <c r="B217" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -3122,31 +3122,31 @@
         <v>211</v>
       </c>
       <c r="B218" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B219" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B220" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="221" spans="1:2">
       <c r="A221" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B221" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -3154,7 +3154,7 @@
         <v>211</v>
       </c>
       <c r="B222" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -3162,6 +3162,14 @@
         <v>211</v>
       </c>
       <c r="B223" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>211</v>
+      </c>
+      <c r="B224" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>